<commit_message>
dictator patch gui clean up
</commit_message>
<xml_diff>
--- a/trade_log.xlsx
+++ b/trade_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O96"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6483,17 +6483,332 @@
       <c r="L96" t="n">
         <v>91435.64</v>
       </c>
-      <c r="M96" t="inlineStr">
+      <c r="M96" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N96" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>dd25c90d-7a65-4bb3-92c5-3f294af53f96</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2025-03-10 13:33:28</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>btcUSDT</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>market_buy</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>82327.60000000001</v>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>futures</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Opened</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Bullish</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>81152.6565</v>
+      </c>
+      <c r="J97" t="n">
+        <v>82184.21904761906</v>
+      </c>
+      <c r="K97" t="n">
+        <v>82201.38571428573</v>
+      </c>
+      <c r="L97" t="n">
+        <v>82220.48000000001</v>
+      </c>
+      <c r="M97" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N97" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>dd25c90d-7a65-4bb3-92c5-3f294af53f96</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2025-03-10 13:33:36</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>btcUSDT</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>market_buy</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>82349.2</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>futures</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Bullish</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>81152.65700000001</v>
+      </c>
+      <c r="J98" t="n">
+        <v>82184.22380952381</v>
+      </c>
+      <c r="K98" t="n">
+        <v>82201.40000000001</v>
+      </c>
+      <c r="L98" t="n">
+        <v>82220.5</v>
+      </c>
+      <c r="M98" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N98" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>c2e6ab33-b3c0-47e4-be70-2344fbc4d023</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2025-03-10 13:33:42</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>btcUSDT</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>market_buy</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>82316.5</v>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>futures</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Opened</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Bullish</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>81152.66</v>
+      </c>
+      <c r="J99" t="n">
+        <v>82184.25238095238</v>
+      </c>
+      <c r="K99" t="n">
+        <v>82201.48571428572</v>
+      </c>
+      <c r="L99" t="n">
+        <v>82220.62</v>
+      </c>
+      <c r="M99" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N99" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>c2e6ab33-b3c0-47e4-be70-2344fbc4d023</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2025-03-10 13:33:48</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>btcUSDT</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>market_buy</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>82357.39999999999</v>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>futures</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Bullish</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>81152.811</v>
+      </c>
+      <c r="J100" t="n">
+        <v>82185.69047619047</v>
+      </c>
+      <c r="K100" t="n">
+        <v>82205.80000000002</v>
+      </c>
+      <c r="L100" t="n">
+        <v>82226.66</v>
+      </c>
+      <c r="M100" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N100" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2e905a54-7391-4929-80f3-05f76ca1d71a</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2025-03-10 18:55:45</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>btcUSDT</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>market_buy</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>82265.5</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>futures</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Opened</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Shortbull</t>
+        </is>
+      </c>
+      <c r="I101" t="n">
+        <v>82298.94</v>
+      </c>
+      <c r="J101" t="n">
+        <v>82226.8142857143</v>
+      </c>
+      <c r="K101" t="n">
+        <v>82256.67142857144</v>
+      </c>
+      <c r="L101" t="n">
+        <v>82269.56</v>
+      </c>
+      <c r="M101" t="inlineStr">
         <is>
           <t>0.02</t>
         </is>
       </c>
-      <c r="N96" t="inlineStr">
+      <c r="N101" t="inlineStr">
         <is>
           <t>0.01</t>
         </is>
       </c>
-      <c r="O96" t="inlineStr">
+      <c r="O101" t="inlineStr">
         <is>
           <t>1m</t>
         </is>

</xml_diff>